<commit_message>
MA_05_02_CO. Corrección de estilo
Con corrección de estilo y ajustes sugeridos.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion02/EsqueletoGuion_MA_05_02_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion02/EsqueletoGuion_MA_05_02_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Planeta\AUTORES\ANDREA\TEMA2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Matematicas\fuentes\contenidos\grado05\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="7230" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20100" windowHeight="7230" tabRatio="729" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -30,42 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>usuario</author>
-  </authors>
-  <commentList>
-    <comment ref="D51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>usuario:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Completar título en corrección de estilo.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="86">
   <si>
     <t>FICHA</t>
   </si>
@@ -247,9 +213,6 @@
     <t>Competencias: construcción de un ábaco chino</t>
   </si>
   <si>
-    <t>En la vida cotidiana, se emplean los números naturales en diferentes contextos: para contar, como código, para ordenar, para representar una cantidad. Conoce equivalencias del sistema decimal con otros sistemas numéricos, operaciones y propiedades de los números naturales.</t>
-  </si>
-  <si>
     <t>El sistema de numeración decimal y sus equivalencias</t>
   </si>
   <si>
@@ -268,9 +231,6 @@
     <t>Aproximación de números naturales por truncamiento</t>
   </si>
   <si>
-    <t>Aproximación por redondeo y por truncamiento en una situación problema</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estimación de resultados </t>
   </si>
   <si>
@@ -322,14 +282,20 @@
     <t>Operaciones combinadas en situaciones problema</t>
   </si>
   <si>
-    <t>Competencias: resolución de situaciones problema que involucran operaciones con números naturales</t>
+    <t>Aproximación por redondeo y truncamiento en una situación problema</t>
+  </si>
+  <si>
+    <t>Competencias: resolución de situaciones problema con operaciones con números naturales</t>
+  </si>
+  <si>
+    <t>En la vida cotidiana se emplean los números naturales en diferentes contextos: para contar, como código, para ordenar, para representar una cantidad. Conoce equivalencias del sistema decimal con otros sistemas numéricos, operaciones y propiedades de los números naturales.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,21 +360,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -436,12 +389,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +845,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -976,35 +923,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1687,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1953,7 +1897,7 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -2264,7 +2208,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
@@ -2274,8 +2218,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
-        <v>67</v>
+      <c r="A3" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>19</v>
@@ -2285,8 +2229,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>70</v>
+      <c r="A4" s="48" t="s">
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>19</v>
@@ -2296,8 +2240,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>77</v>
+      <c r="A5" s="48" t="s">
+        <v>75</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>19</v>
@@ -2307,8 +2251,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>81</v>
+      <c r="A6" s="48" t="s">
+        <v>79</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>19</v>
@@ -2318,8 +2262,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>82</v>
+      <c r="A7" s="48" t="s">
+        <v>80</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
@@ -2329,8 +2273,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>84</v>
+      <c r="A8" s="48" t="s">
+        <v>82</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
@@ -2340,8 +2284,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>85</v>
+      <c r="A9" s="48" t="s">
+        <v>84</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>19</v>
@@ -2566,7 +2510,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -2587,8 +2531,8 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>67</v>
+      <c r="B10" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2599,7 +2543,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
@@ -2610,7 +2554,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -2676,7 +2620,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -2720,7 +2664,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2742,7 +2686,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2775,7 +2719,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>19</v>
@@ -2807,8 +2751,8 @@
       <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="29" t="s">
-        <v>85</v>
+      <c r="B30" s="48" t="s">
+        <v>84</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>19</v>
@@ -2857,11 +2801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="E65" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,25 +2919,19 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
-      <c r="H6" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>24</v>
-      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
@@ -3003,14 +2941,18 @@
         <v>39</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="D7" s="27"/>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="H7" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
@@ -3020,11 +2962,11 @@
         <v>39</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="27"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -3037,18 +2979,14 @@
         <v>39</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="32"/>
       <c r="F9" s="27"/>
       <c r="G9" s="32"/>
-      <c r="H9" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>24</v>
-      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
@@ -3057,17 +2995,19 @@
       <c r="B10" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>25</v>
-      </c>
+      <c r="C10" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="27"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
+      <c r="H10" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
@@ -3077,22 +3017,18 @@
         <v>39</v>
       </c>
       <c r="C11" s="27"/>
-      <c r="D11" s="49" t="s">
-        <v>61</v>
+      <c r="D11" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="32"/>
-      <c r="H11" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>39</v>
       </c>
@@ -3100,16 +3036,20 @@
         <v>39</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="27" t="s">
-        <v>62</v>
+      <c r="D12" s="47" t="s">
+        <v>60</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
+      <c r="H12" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
@@ -3120,12 +3060,12 @@
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="32"/>
+        <v>25</v>
+      </c>
+      <c r="F13" s="27"/>
       <c r="G13" s="32"/>
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
@@ -3139,13 +3079,13 @@
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
     </row>
@@ -3158,15 +3098,15 @@
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="31"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
@@ -3177,10 +3117,10 @@
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
@@ -3196,10 +3136,10 @@
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
@@ -3215,10 +3155,10 @@
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
@@ -3234,15 +3174,15 @@
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
@@ -3253,19 +3193,15 @@
       </c>
       <c r="C20" s="27"/>
       <c r="D20" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
-      <c r="H20" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="31" t="s">
-        <v>24</v>
-      </c>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
@@ -3276,15 +3212,15 @@
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
       <c r="H21" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I21" s="31" t="s">
         <v>24</v>
@@ -3299,7 +3235,7 @@
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>28</v>
@@ -3307,7 +3243,7 @@
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
       <c r="H22" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I22" s="31" t="s">
         <v>24</v>
@@ -3322,7 +3258,7 @@
       </c>
       <c r="C23" s="27"/>
       <c r="D23" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="30" t="s">
         <v>28</v>
@@ -3330,13 +3266,13 @@
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
       <c r="H23" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>39</v>
       </c>
@@ -3345,15 +3281,19 @@
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="30"/>
+      <c r="H24" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
@@ -3362,18 +3302,16 @@
       <c r="B25" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="30"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="35"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="30"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3385,19 +3323,19 @@
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="30"/>
       <c r="F26" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="31"/>
+        <v>25</v>
+      </c>
+      <c r="H26" s="35"/>
       <c r="I26" s="30"/>
     </row>
-    <row r="27" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>39</v>
       </c>
@@ -3406,23 +3344,19 @@
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H27" s="31"/>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>39</v>
       </c>
@@ -3431,19 +3365,23 @@
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="36" t="s">
-        <v>66</v>
-      </c>
       <c r="G28" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="30"/>
-    </row>
-    <row r="29" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>39</v>
       </c>
@@ -3452,23 +3390,19 @@
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="30"/>
       <c r="F29" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H29" s="31"/>
+      <c r="I29" s="30"/>
+    </row>
+    <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>39</v>
       </c>
@@ -3477,15 +3411,21 @@
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+        <v>63</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
@@ -3496,15 +3436,15 @@
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="31"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
@@ -3515,19 +3455,15 @@
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
-      <c r="H32" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>24</v>
-      </c>
+      <c r="H32" s="35"/>
+      <c r="I32" s="31"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
@@ -3538,7 +3474,7 @@
       </c>
       <c r="C33" s="30"/>
       <c r="D33" s="27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="30" t="s">
         <v>28</v>
@@ -3546,10 +3482,10 @@
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
       <c r="H33" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I33" s="30" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3561,15 +3497,19 @@
       </c>
       <c r="C34" s="30"/>
       <c r="D34" s="27" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
+      <c r="H34" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="30" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="30" t="s">
@@ -3583,48 +3523,48 @@
         <v>31</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="I35" s="30" t="s">
+      <c r="I36" s="30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="16" t="s">
         <v>25</v>
       </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
@@ -3635,14 +3575,14 @@
         <v>39</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
@@ -3654,18 +3594,18 @@
         <v>39</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" s="16"/>
       <c r="D39" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="21"/>
+      <c r="H39" s="16"/>
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3673,83 +3613,81 @@
         <v>39</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C40" s="16"/>
       <c r="D40" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" s="39"/>
+        <v>25</v>
+      </c>
+      <c r="F40" s="16"/>
       <c r="G40" s="16"/>
-      <c r="H40" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="H40" s="21"/>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" s="16"/>
       <c r="D41" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="39"/>
+        <v>28</v>
+      </c>
+      <c r="F41" s="37"/>
       <c r="G41" s="16"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="16"/>
+      <c r="H41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="18"/>
+        <v>69</v>
+      </c>
+      <c r="C42" s="16"/>
       <c r="D42" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="G42" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H42" s="16"/>
-      <c r="I42" s="18"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E43" s="18"/>
-      <c r="F43" s="39" t="s">
-        <v>74</v>
+      <c r="F43" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H43" s="21"/>
+      <c r="H43" s="16"/>
       <c r="I43" s="18"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3757,20 +3695,20 @@
         <v>39</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="18" t="s">
+      <c r="G44" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="H44" s="18"/>
+      <c r="H44" s="21"/>
       <c r="I44" s="18"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3778,46 +3716,42 @@
         <v>39</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E45" s="18"/>
-      <c r="F45" s="39" t="s">
-        <v>75</v>
+      <c r="F45" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I45" s="18" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E46" s="18"/>
-      <c r="F46" s="39" t="s">
-        <v>75</v>
+      <c r="F46" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I46" s="18" t="s">
         <v>24</v>
@@ -3828,37 +3762,43 @@
         <v>39</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="E47" s="18"/>
+      <c r="F47" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
-      <c r="H48" s="22"/>
+      <c r="H48" s="18"/>
       <c r="I48" s="18"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,38 +3806,30 @@
         <v>39</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>25</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C49" s="18"/>
       <c r="D49" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F49" s="18"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="I49" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="G49" s="18"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="18"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>27</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C50" s="18"/>
       <c r="D50" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>28</v>
@@ -3905,10 +3837,10 @@
       <c r="F50" s="18"/>
       <c r="G50" s="21"/>
       <c r="H50" s="22" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="I50" s="18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3916,84 +3848,82 @@
         <v>39</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="38" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F51" s="18"/>
       <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="18"/>
+      <c r="H51" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D52" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>28</v>
-      </c>
       <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I52" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="18"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C53" s="18"/>
-      <c r="D53" s="38" t="s">
-        <v>80</v>
+      <c r="D53" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
+      <c r="H53" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I53" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" s="18"/>
-      <c r="D54" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="G54" s="18" t="s">
+      <c r="D54" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="18" t="s">
         <v>25</v>
       </c>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
       <c r="H54" s="18"/>
       <c r="I54" s="18"/>
     </row>
@@ -4002,15 +3932,15 @@
         <v>39</v>
       </c>
       <c r="B55" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="18"/>
+      <c r="F55" s="37" t="s">
         <v>71</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="39" t="s">
-        <v>74</v>
       </c>
       <c r="G55" s="18" t="s">
         <v>25</v>
@@ -4023,15 +3953,15 @@
         <v>39</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C56" s="18"/>
-      <c r="D56" s="38" t="s">
-        <v>80</v>
+      <c r="D56" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="E56" s="18"/>
-      <c r="F56" s="39" t="s">
-        <v>75</v>
+      <c r="F56" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="G56" s="18" t="s">
         <v>25</v>
@@ -4039,25 +3969,25 @@
       <c r="H56" s="18"/>
       <c r="I56" s="18"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E57" s="18"/>
-      <c r="F57" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G57" s="22" t="s">
+      <c r="F57" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H57" s="22"/>
+      <c r="H57" s="18"/>
       <c r="I57" s="18"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4065,158 +3995,156 @@
         <v>39</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E58" s="18"/>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" s="22"/>
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G58" s="22" t="s">
+      <c r="E59" s="18"/>
+      <c r="F59" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I58" s="18" t="s">
+      <c r="I59" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E59" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="23"/>
     </row>
     <row r="60" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" s="18"/>
+        <v>69</v>
+      </c>
+      <c r="C60" s="23"/>
       <c r="D60" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F60" s="18"/>
+        <v>77</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="20"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
-      <c r="I60" s="18"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I60" s="23"/>
+    </row>
+    <row r="61" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F61" s="18"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I61" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H61" s="22"/>
+      <c r="I61" s="18"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E62" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="22"/>
       <c r="H62" s="22" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C63" s="18"/>
-      <c r="D63" s="16" t="s">
-        <v>31</v>
+      <c r="D63" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F63" s="16"/>
       <c r="G63" s="16"/>
-      <c r="H63" s="22"/>
-      <c r="I63" s="18"/>
+      <c r="H63" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C64" s="18"/>
-      <c r="D64" s="21" t="s">
+      <c r="D64" s="16" t="s">
         <v>31</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F64" s="16"/>
       <c r="G64" s="16"/>
-      <c r="H64" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I64" s="18" t="s">
-        <v>24</v>
-      </c>
+      <c r="H64" s="22"/>
+      <c r="I64" s="18"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="21" t="s">
@@ -4228,246 +4156,258 @@
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
       <c r="H65" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I65" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="18"/>
+      <c r="D66" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I66" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" s="40"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="41"/>
+    </row>
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="40"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I68" s="41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="40"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="I69" s="41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" s="40"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="39"/>
+      <c r="H70" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I65" s="18" t="s">
+      <c r="I70" s="41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B66" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="43" t="s">
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="41"/>
+      <c r="D71" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E71" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="42"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="43"/>
-    </row>
-    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B67" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C67" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" s="42"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="41"/>
-      <c r="G67" s="41"/>
-      <c r="H67" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="I67" s="43" t="s">
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="42"/>
+      <c r="I71" s="41"/>
+    </row>
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="41"/>
+      <c r="D72" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F72" s="39"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="I72" s="41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B68" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C68" s="43" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="46"/>
+      <c r="E73" s="46"/>
+      <c r="F73" s="46"/>
+      <c r="G73" s="45"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="46"/>
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D68" s="42"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="41"/>
-      <c r="H68" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="I68" s="43" t="s">
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="I74" s="46" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B69" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C69" s="43" t="s">
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="42"/>
-      <c r="E69" s="41"/>
-      <c r="F69" s="41"/>
-      <c r="G69" s="41"/>
-      <c r="H69" s="44" t="s">
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="I69" s="43" t="s">
+      <c r="I75" s="46" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B70" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="E70" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
-      <c r="H70" s="44"/>
-      <c r="I70" s="43"/>
-    </row>
-    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B71" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="E71" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="F71" s="41"/>
-      <c r="G71" s="41"/>
-      <c r="H71" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="I71" s="43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C72" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="4"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B73" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C73" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="47"/>
-      <c r="H73" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="I73" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="J73" s="4"/>
-    </row>
-    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B74" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C74" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="I74" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="J74" s="4"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B75" s="47" t="s">
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B76" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="48" t="s">
+      <c r="C76" s="46" t="s">
         <v>33</v>
-      </c>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="J75" s="4"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B76" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="46" t="s">
-        <v>34</v>
       </c>
       <c r="D76" s="46"/>
       <c r="E76" s="46"/>
       <c r="F76" s="46"/>
-      <c r="G76" s="46"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="48" t="s">
+      <c r="G76" s="45"/>
+      <c r="H76" s="45"/>
+      <c r="I76" s="46" t="s">
         <v>19</v>
       </c>
       <c r="J76" s="4"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
-      <c r="H77" s="22"/>
-      <c r="I77" s="18"/>
+      <c r="A77" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B77" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="J77" s="4"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
@@ -4482,14 +4422,14 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="16"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="18"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="16"/>
@@ -4502,10 +4442,20 @@
       <c r="H80" s="24"/>
       <c r="I80" s="24"/>
     </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="16"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>